<commit_message>
Add schematic and sources folder/files (see if windows format rise issue)
</commit_message>
<xml_diff>
--- a/Calcul.xlsx
+++ b/Calcul.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Electronique\POV_Clock\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7921A8C8-00FD-4A40-A20F-93C9B56EFFB9}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AFD6419A-65BA-4D99-BFF2-81C727175460}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1290" yWindow="1530" windowWidth="27465" windowHeight="13620" xr2:uid="{2F3C8286-4817-4693-8521-6FB3783A5BD8}"/>
+    <workbookView xWindow="390" yWindow="390" windowWidth="38700" windowHeight="15435" xr2:uid="{2F3C8286-4817-4693-8521-6FB3783A5BD8}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
   <si>
     <t>Vitesse tr/min</t>
   </si>
@@ -91,6 +91,9 @@
   </si>
   <si>
     <t>densité [g/cm3]</t>
+  </si>
+  <si>
+    <t>test</t>
   </si>
 </sst>
 </file>
@@ -452,10 +455,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{434C2399-E884-4BC9-B03D-F2E7013DEC0F}">
-  <dimension ref="A1:J12"/>
+  <dimension ref="A1:J13"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="M15" sqref="M15"/>
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -589,6 +592,11 @@
         <v>4.8309178743961353E-6</v>
       </c>
     </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>20</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>